<commit_message>
Actualizacion final dell Diccionario de Datos
</commit_message>
<xml_diff>
--- a/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
+++ b/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{873D2478-7A96-4631-878A-2EB765DC6240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42395F3B-57F7-4BF6-9BE2-7D0EA45AC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F443A80F-953F-496B-8468-B3E2331811A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="161">
   <si>
     <t>Tabla Origen</t>
   </si>
@@ -137,9 +137,6 @@
     <t>es_activo</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t>creado_por</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>id_subcategoria</t>
   </si>
   <si>
-    <t>id_padre</t>
-  </si>
-  <si>
     <t>detalles_presupuesto</t>
   </si>
   <si>
@@ -254,9 +248,6 @@
     <t>id_obligacion</t>
   </si>
   <si>
-    <t>id_dueno</t>
-  </si>
-  <si>
     <t>monto_fijo</t>
   </si>
   <si>
@@ -308,9 +299,6 @@
     <t>comentarios_extra</t>
   </si>
   <si>
-    <t>fecha_hora_transaccion</t>
-  </si>
-  <si>
     <t>fecha_transaccion</t>
   </si>
   <si>
@@ -494,9 +482,6 @@
     <t>Texto de comentarios extra para la transaccion (opcional)</t>
   </si>
   <si>
-    <t>Fecha con la hora de la transaccion</t>
-  </si>
-  <si>
     <t>Identificador unico de la meta de ahorro</t>
   </si>
   <si>
@@ -522,6 +507,18 @@
   </si>
   <si>
     <t>Estado actual de la meta de ahorro</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>fecha_hora_registro</t>
+  </si>
+  <si>
+    <t>Fecha y hora de registro en el sistema</t>
   </si>
 </sst>
 </file>
@@ -586,13 +583,65 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}"/>
+  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}">
+    <filterColumn colId="1">
+      <filters blank="1">
+        <filter val="anio_final"/>
+        <filter val="anio_inicio"/>
+        <filter val="anio_transaccion"/>
+        <filter val="apellidos"/>
+        <filter val="color"/>
+        <filter val="comentarios_extra"/>
+        <filter val="correo_electronico"/>
+        <filter val="descripcion"/>
+        <filter val="dia_vencimiento"/>
+        <filter val="es_activo"/>
+        <filter val="es_predeterminado"/>
+        <filter val="es_vigente"/>
+        <filter val="estado"/>
+        <filter val="fecha_creacion"/>
+        <filter val="fecha_final"/>
+        <filter val="fecha_hora_transaccion"/>
+        <filter val="fecha_inicio"/>
+        <filter val="fecha_objetivo"/>
+        <filter val="fecha_registro"/>
+        <filter val="fecha_transaccion"/>
+        <filter val="id_categoria"/>
+        <filter val="id_detalle"/>
+        <filter val="id_dueno"/>
+        <filter val="id_meta"/>
+        <filter val="id_obligacion"/>
+        <filter val="id_presupuesto"/>
+        <filter val="id_subcategoria"/>
+        <filter val="id_transaccion"/>
+        <filter val="id_usuario"/>
+        <filter val="justificacion"/>
+        <filter val="mes_final"/>
+        <filter val="mes_inicio"/>
+        <filter val="mes_transaccion"/>
+        <filter val="metodo_pago"/>
+        <filter val="monto"/>
+        <filter val="monto_ahorrado"/>
+        <filter val="monto_asignado"/>
+        <filter val="monto_fijo"/>
+        <filter val="monto_meta"/>
+        <filter val="nombre"/>
+        <filter val="nombre_icono"/>
+        <filter val="nombre_presupuesto"/>
+        <filter val="nombres"/>
+        <filter val="numero_factura"/>
+        <filter val="orden_interfaz"/>
+        <filter val="prioridad"/>
+        <filter val="salario_base"/>
+        <filter val="tipo_categoria"/>
+        <filter val="tipo_transaccion"/>
+        <filter val="total_gastos"/>
+        <filter val="total_ingresos"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{73440C09-8613-4802-8EE4-A5004834AFD1}" name="Tabla Origen"/>
     <tableColumn id="2" xr3:uid="{74162E37-FF63-4757-8E2F-B0116BA80DA9}" name="Nombre de Columna"/>
@@ -925,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E7A639-BE3C-43E1-8C0C-70E76DACB4DD}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,22 +1133,24 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -1112,12 +1163,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -1130,15 +1181,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1148,15 +1199,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1168,10 +1219,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1184,36 +1235,36 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -1223,15 +1274,15 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1241,15 +1292,15 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1258,18 +1309,18 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1279,15 +1330,15 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1296,18 +1347,18 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -1317,15 +1368,15 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1335,15 +1386,15 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -1353,12 +1404,12 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
@@ -1370,18 +1421,18 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1394,12 +1445,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1412,15 +1463,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1430,15 +1481,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
         <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1450,10 +1501,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1466,15 +1517,15 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1484,15 +1535,15 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1502,15 +1553,15 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1519,18 +1570,18 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1540,15 +1591,15 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1557,18 +1608,18 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1578,15 +1629,15 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -1599,12 +1650,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -1617,15 +1668,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1635,15 +1686,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
         <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -1655,10 +1706,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
         <v>63</v>
-      </c>
-      <c r="B39" t="s">
-        <v>64</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1671,15 +1722,15 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1688,19 +1739,19 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -1710,15 +1761,15 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -1728,51 +1779,55 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G43" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
         <v>33</v>
-      </c>
-      <c r="D44" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" t="s">
-        <v>34</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -1785,12 +1840,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -1803,15 +1858,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -1821,15 +1876,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" t="s">
         <v>37</v>
-      </c>
-      <c r="C48" t="s">
-        <v>38</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -1841,10 +1896,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1857,15 +1912,15 @@
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
@@ -1874,19 +1929,19 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1895,19 +1950,19 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
         <v>66</v>
-      </c>
-      <c r="B52" t="s">
-        <v>68</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -1917,15 +1972,15 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -1935,15 +1990,15 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -1956,12 +2011,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -1974,15 +2029,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -1992,15 +2047,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
         <v>37</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2012,10 +2067,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -2028,15 +2083,15 @@
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -2045,19 +2100,19 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2066,19 +2121,19 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -2088,15 +2143,15 @@
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -2106,15 +2161,15 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="s">
         <v>70</v>
-      </c>
-      <c r="B63" t="s">
-        <v>73</v>
       </c>
       <c r="C63" t="s">
         <v>30</v>
@@ -2124,15 +2179,15 @@
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -2141,36 +2196,38 @@
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G65" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C66" t="s">
         <v>29</v>
@@ -2180,33 +2237,33 @@
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
         <v>29</v>
       </c>
       <c r="D67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C68" t="s">
         <v>23</v>
@@ -2219,12 +2276,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
@@ -2237,15 +2294,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2255,15 +2312,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" t="s">
         <v>37</v>
-      </c>
-      <c r="C71" t="s">
-        <v>38</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2275,13 +2332,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2291,15 +2348,15 @@
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
@@ -2308,19 +2365,19 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -2329,37 +2386,37 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
         <v>79</v>
-      </c>
-      <c r="B76" t="s">
-        <v>82</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -2368,18 +2425,18 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -2388,40 +2445,40 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C78" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
         <v>23</v>
@@ -2430,18 +2487,18 @@
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C80" t="s">
         <v>23</v>
@@ -2451,15 +2508,15 @@
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
         <v>30</v>
@@ -2469,15 +2526,15 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C82" t="s">
         <v>29</v>
@@ -2487,15 +2544,15 @@
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C83" t="s">
         <v>23</v>
@@ -2504,18 +2561,18 @@
         <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -2525,15 +2582,15 @@
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C85" t="s">
         <v>23</v>
@@ -2543,33 +2600,33 @@
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="C86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B87" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C87" t="s">
         <v>23</v>
@@ -2582,12 +2639,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
@@ -2600,15 +2657,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C89" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -2618,15 +2675,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B90" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" t="s">
         <v>37</v>
-      </c>
-      <c r="C90" t="s">
-        <v>38</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -2638,10 +2695,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
@@ -2654,15 +2711,15 @@
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
@@ -2671,19 +2728,19 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2692,19 +2749,19 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C94" t="s">
         <v>23</v>
@@ -2714,15 +2771,15 @@
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
@@ -2732,15 +2789,15 @@
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C96" t="s">
         <v>30</v>
@@ -2750,15 +2807,15 @@
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
         <v>30</v>
@@ -2768,15 +2825,15 @@
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C98" t="s">
         <v>29</v>
@@ -2786,15 +2843,15 @@
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" t="s">
         <v>92</v>
-      </c>
-      <c r="B99" t="s">
-        <v>96</v>
       </c>
       <c r="C99" t="s">
         <v>29</v>
@@ -2804,15 +2861,15 @@
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B100" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C100" t="s">
         <v>23</v>
@@ -2821,15 +2878,15 @@
         <v>0</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B101" t="s">
         <v>31</v>
@@ -2841,18 +2898,18 @@
         <v>0</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
@@ -2865,12 +2922,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -2883,15 +2940,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C104" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -2901,15 +2958,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B105" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" t="s">
         <v>37</v>
-      </c>
-      <c r="C105" t="s">
-        <v>38</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -2995,15 +3052,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010059BC34D888E3A3459199F7DD1A29DC10" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a167d785635a8e7b15aad71fca406d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="76cacb90-fab5-4ebd-b504-b341093fce80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41504c81f65ced929038d69d6343efbf" ns3:_="">
     <xsd:import namespace="76cacb90-fab5-4ebd-b504-b341093fce80"/>
@@ -3153,6 +3201,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
   <ds:schemaRefs>
@@ -3170,14 +3227,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{579D9562-EB3A-4EB6-9BAA-4CEE18FA3F82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3193,4 +3242,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambios a la creacion de tablas usando create or replace, y correcciones para el diccionario de datos
</commit_message>
<xml_diff>
--- a/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
+++ b/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto_Presupuesto\proyecto-presupuesto-personal\Q4Projecto-Presupuesto-Personal-Mensual\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42395F3B-57F7-4BF6-9BE2-7D0EA45AC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4323C-F20A-4EAB-BAE1-8D2BC0FBDB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F443A80F-953F-496B-8468-B3E2331811A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="162">
   <si>
     <t>Tabla Origen</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>Fecha y hora de registro en el sistema</t>
+  </si>
+  <si>
+    <t>Descripcion del proyecto</t>
   </si>
 </sst>
 </file>
@@ -585,63 +588,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}">
-    <filterColumn colId="1">
-      <filters blank="1">
-        <filter val="anio_final"/>
-        <filter val="anio_inicio"/>
-        <filter val="anio_transaccion"/>
-        <filter val="apellidos"/>
-        <filter val="color"/>
-        <filter val="comentarios_extra"/>
-        <filter val="correo_electronico"/>
-        <filter val="descripcion"/>
-        <filter val="dia_vencimiento"/>
-        <filter val="es_activo"/>
-        <filter val="es_predeterminado"/>
-        <filter val="es_vigente"/>
-        <filter val="estado"/>
-        <filter val="fecha_creacion"/>
-        <filter val="fecha_final"/>
-        <filter val="fecha_hora_transaccion"/>
-        <filter val="fecha_inicio"/>
-        <filter val="fecha_objetivo"/>
-        <filter val="fecha_registro"/>
-        <filter val="fecha_transaccion"/>
-        <filter val="id_categoria"/>
-        <filter val="id_detalle"/>
-        <filter val="id_dueno"/>
-        <filter val="id_meta"/>
-        <filter val="id_obligacion"/>
-        <filter val="id_presupuesto"/>
-        <filter val="id_subcategoria"/>
-        <filter val="id_transaccion"/>
-        <filter val="id_usuario"/>
-        <filter val="justificacion"/>
-        <filter val="mes_final"/>
-        <filter val="mes_inicio"/>
-        <filter val="mes_transaccion"/>
-        <filter val="metodo_pago"/>
-        <filter val="monto"/>
-        <filter val="monto_ahorrado"/>
-        <filter val="monto_asignado"/>
-        <filter val="monto_fijo"/>
-        <filter val="monto_meta"/>
-        <filter val="nombre"/>
-        <filter val="nombre_icono"/>
-        <filter val="nombre_presupuesto"/>
-        <filter val="nombres"/>
-        <filter val="numero_factura"/>
-        <filter val="orden_interfaz"/>
-        <filter val="prioridad"/>
-        <filter val="salario_base"/>
-        <filter val="tipo_categoria"/>
-        <filter val="tipo_transaccion"/>
-        <filter val="total_gastos"/>
-        <filter val="total_ingresos"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{73440C09-8613-4802-8EE4-A5004834AFD1}" name="Tabla Origen"/>
     <tableColumn id="2" xr3:uid="{74162E37-FF63-4757-8E2F-B0116BA80DA9}" name="Nombre de Columna"/>
@@ -974,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E7A639-BE3C-43E1-8C0C-70E76DACB4DD}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1282,17 +1229,17 @@
         <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,7 +1247,7 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1308,11 +1255,9 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,7 +1265,7 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1328,9 +1273,11 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1338,7 +1285,7 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1346,29 +1293,29 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1376,7 +1323,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1386,53 +1333,51 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1440,17 +1385,19 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1460,33 +1407,33 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -1496,28 +1443,25 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1525,17 +1469,20 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1543,7 +1490,7 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1553,15 +1500,15 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1569,11 +1516,9 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1581,25 +1526,27 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G32" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1607,55 +1554,55 @@
       <c r="D33" t="b">
         <v>1</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G34" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -1665,33 +1612,33 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1701,28 +1648,25 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1730,7 +1674,7 @@
         <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1739,11 +1683,11 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,17 +1695,20 @@
         <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,7 +1716,7 @@
         <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -1779,7 +1726,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1787,27 +1734,25 @@
         <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
         <v>157</v>
@@ -1819,33 +1764,35 @@
         <v>158</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -1855,33 +1802,33 @@
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -1891,36 +1838,33 @@
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
@@ -1929,11 +1873,11 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1941,7 +1885,7 @@
         <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1954,25 +1898,28 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,25 +1927,25 @@
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -2008,15 +1955,15 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -2026,33 +1973,33 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
@@ -2062,28 +2009,25 @@
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>10</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2091,7 +2035,7 @@
         <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -2100,19 +2044,19 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2125,25 +2069,28 @@
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>50</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,7 +2098,7 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -2161,7 +2108,7 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2169,17 +2116,17 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2187,19 +2134,17 @@
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,19 +2152,19 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,17 +2172,19 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G66" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2245,43 +2192,43 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
         <v>29</v>
       </c>
       <c r="D67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
@@ -2291,33 +2238,33 @@
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C71" t="s">
         <v>37</v>
@@ -2327,28 +2274,25 @@
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>10</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2356,28 +2300,28 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -2390,25 +2334,28 @@
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>50</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2416,27 +2363,25 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -2444,12 +2389,11 @@
       <c r="D77" t="b">
         <v>0</v>
       </c>
-      <c r="E77" t="s">
-        <v>50</v>
-      </c>
-      <c r="F77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G77" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2457,20 +2401,20 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C78" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" t="s">
         <v>50</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2478,27 +2422,28 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D79" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C80" t="s">
         <v>23</v>
@@ -2506,9 +2451,11 @@
       <c r="D80" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G80" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2516,17 +2463,17 @@
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2534,117 +2481,117 @@
         <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D84" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G84" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C85" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="C86" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>76</v>
       </c>
       <c r="B87" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
@@ -2654,33 +2601,33 @@
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
         <v>37</v>
@@ -2690,28 +2637,25 @@
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
-      </c>
-      <c r="E91" t="s">
-        <v>10</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,7 +2663,7 @@
         <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
@@ -2728,19 +2672,19 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2753,25 +2697,28 @@
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C94" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>50</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2779,7 +2726,7 @@
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
@@ -2789,7 +2736,7 @@
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2797,25 +2744,25 @@
         <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97" t="s">
         <v>30</v>
@@ -2825,33 +2772,33 @@
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
         <v>29</v>
@@ -2861,7 +2808,7 @@
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2869,27 +2816,25 @@
         <v>88</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C100" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>88</v>
       </c>
       <c r="B101" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C101" t="s">
         <v>23</v>
@@ -2898,18 +2843,18 @@
         <v>0</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
@@ -2917,17 +2862,19 @@
       <c r="D102" t="b">
         <v>0</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="G102" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -2937,33 +2884,33 @@
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C104" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>88</v>
       </c>
       <c r="B105" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C105" t="s">
         <v>37</v>
@@ -2973,12 +2920,26 @@
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>88</v>
+      </c>
+      <c r="B106" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F107" s="1"/>
@@ -3046,9 +3007,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3202,26 +3166,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3245,9 +3198,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificaciones al diccionario de datos y crear tablas
</commit_message>
<xml_diff>
--- a/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
+++ b/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto_Presupuesto\proyecto-presupuesto-personal\Q4Projecto-Presupuesto-Personal-Mensual\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42395F3B-57F7-4BF6-9BE2-7D0EA45AC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4323C-F20A-4EAB-BAE1-8D2BC0FBDB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F443A80F-953F-496B-8468-B3E2331811A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="162">
   <si>
     <t>Tabla Origen</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>Fecha y hora de registro en el sistema</t>
+  </si>
+  <si>
+    <t>Descripcion del proyecto</t>
   </si>
 </sst>
 </file>
@@ -585,63 +588,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}">
-    <filterColumn colId="1">
-      <filters blank="1">
-        <filter val="anio_final"/>
-        <filter val="anio_inicio"/>
-        <filter val="anio_transaccion"/>
-        <filter val="apellidos"/>
-        <filter val="color"/>
-        <filter val="comentarios_extra"/>
-        <filter val="correo_electronico"/>
-        <filter val="descripcion"/>
-        <filter val="dia_vencimiento"/>
-        <filter val="es_activo"/>
-        <filter val="es_predeterminado"/>
-        <filter val="es_vigente"/>
-        <filter val="estado"/>
-        <filter val="fecha_creacion"/>
-        <filter val="fecha_final"/>
-        <filter val="fecha_hora_transaccion"/>
-        <filter val="fecha_inicio"/>
-        <filter val="fecha_objetivo"/>
-        <filter val="fecha_registro"/>
-        <filter val="fecha_transaccion"/>
-        <filter val="id_categoria"/>
-        <filter val="id_detalle"/>
-        <filter val="id_dueno"/>
-        <filter val="id_meta"/>
-        <filter val="id_obligacion"/>
-        <filter val="id_presupuesto"/>
-        <filter val="id_subcategoria"/>
-        <filter val="id_transaccion"/>
-        <filter val="id_usuario"/>
-        <filter val="justificacion"/>
-        <filter val="mes_final"/>
-        <filter val="mes_inicio"/>
-        <filter val="mes_transaccion"/>
-        <filter val="metodo_pago"/>
-        <filter val="monto"/>
-        <filter val="monto_ahorrado"/>
-        <filter val="monto_asignado"/>
-        <filter val="monto_fijo"/>
-        <filter val="monto_meta"/>
-        <filter val="nombre"/>
-        <filter val="nombre_icono"/>
-        <filter val="nombre_presupuesto"/>
-        <filter val="nombres"/>
-        <filter val="numero_factura"/>
-        <filter val="orden_interfaz"/>
-        <filter val="prioridad"/>
-        <filter val="salario_base"/>
-        <filter val="tipo_categoria"/>
-        <filter val="tipo_transaccion"/>
-        <filter val="total_gastos"/>
-        <filter val="total_ingresos"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G1048576" xr:uid="{64F77E5A-A87D-4765-AED6-65DB5CA2FC16}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{73440C09-8613-4802-8EE4-A5004834AFD1}" name="Tabla Origen"/>
     <tableColumn id="2" xr3:uid="{74162E37-FF63-4757-8E2F-B0116BA80DA9}" name="Nombre de Columna"/>
@@ -974,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E7A639-BE3C-43E1-8C0C-70E76DACB4DD}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1282,17 +1229,17 @@
         <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,7 +1247,7 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1308,11 +1255,9 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,7 +1265,7 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1328,9 +1273,11 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1338,7 +1285,7 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1346,29 +1293,29 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1376,7 +1323,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1386,53 +1333,51 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1440,17 +1385,19 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1460,33 +1407,33 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -1496,28 +1443,25 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1525,17 +1469,20 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1543,7 +1490,7 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1553,15 +1500,15 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1569,11 +1516,9 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1581,25 +1526,27 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G32" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1607,55 +1554,55 @@
       <c r="D33" t="b">
         <v>1</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G34" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -1665,33 +1612,33 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1701,28 +1648,25 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1730,7 +1674,7 @@
         <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1739,11 +1683,11 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,17 +1695,20 @@
         <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,7 +1716,7 @@
         <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -1779,7 +1726,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1787,27 +1734,25 @@
         <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
         <v>157</v>
@@ -1819,33 +1764,35 @@
         <v>158</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -1855,33 +1802,33 @@
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -1891,36 +1838,33 @@
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
@@ -1929,11 +1873,11 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1941,7 +1885,7 @@
         <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1954,25 +1898,28 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,25 +1927,25 @@
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -2008,15 +1955,15 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -2026,33 +1973,33 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
@@ -2062,28 +2009,25 @@
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>10</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2091,7 +2035,7 @@
         <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -2100,19 +2044,19 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2125,25 +2069,28 @@
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>50</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,7 +2098,7 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -2161,7 +2108,7 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2169,17 +2116,17 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2187,19 +2134,17 @@
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,19 +2152,19 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,17 +2172,19 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G66" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2245,43 +2192,43 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
         <v>29</v>
       </c>
       <c r="D67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
@@ -2291,33 +2238,33 @@
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C71" t="s">
         <v>37</v>
@@ -2327,28 +2274,25 @@
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>10</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2356,28 +2300,28 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -2390,25 +2334,28 @@
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>50</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2416,27 +2363,25 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -2444,12 +2389,11 @@
       <c r="D77" t="b">
         <v>0</v>
       </c>
-      <c r="E77" t="s">
-        <v>50</v>
-      </c>
-      <c r="F77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G77" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2457,20 +2401,20 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C78" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" t="s">
         <v>50</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2478,27 +2422,28 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D79" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C80" t="s">
         <v>23</v>
@@ -2506,9 +2451,11 @@
       <c r="D80" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G80" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2516,17 +2463,17 @@
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2534,117 +2481,117 @@
         <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D84" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G84" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C85" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="C86" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>76</v>
       </c>
       <c r="B87" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
@@ -2654,33 +2601,33 @@
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
         <v>37</v>
@@ -2690,28 +2637,25 @@
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
-      </c>
-      <c r="E91" t="s">
-        <v>10</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,7 +2663,7 @@
         <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
@@ -2728,19 +2672,19 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2753,25 +2697,28 @@
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C94" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>50</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2779,7 +2726,7 @@
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
@@ -2789,7 +2736,7 @@
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2797,25 +2744,25 @@
         <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97" t="s">
         <v>30</v>
@@ -2825,33 +2772,33 @@
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
         <v>29</v>
@@ -2861,7 +2808,7 @@
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2869,27 +2816,25 @@
         <v>88</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C100" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>88</v>
       </c>
       <c r="B101" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C101" t="s">
         <v>23</v>
@@ -2898,18 +2843,18 @@
         <v>0</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
@@ -2917,17 +2862,19 @@
       <c r="D102" t="b">
         <v>0</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="G102" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -2937,33 +2884,33 @@
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C104" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>88</v>
       </c>
       <c r="B105" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C105" t="s">
         <v>37</v>
@@ -2973,12 +2920,26 @@
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>88</v>
+      </c>
+      <c r="B106" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F107" s="1"/>
@@ -3046,9 +3007,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3202,26 +3166,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3245,9 +3198,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambio al diccionario de datos y crear_tabla + agregar el primer procedimiento de negocio
Pequeño cambio al diccionario de datos y crear tabla + agregar el primer procedimiento de negocio
</commit_message>
<xml_diff>
--- a/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
+++ b/Q4Projecto-Presupuesto-Personal-Mensual/docs/DiccionarioDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto_Presupuesto\proyecto-presupuesto-personal\Q4Projecto-Presupuesto-Personal-Mensual\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4323C-F20A-4EAB-BAE1-8D2BC0FBDB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5DD9CC-378C-49B3-9F13-8C026AA03A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F443A80F-953F-496B-8468-B3E2331811A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="164">
   <si>
     <t>Tabla Origen</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>Descripcion del proyecto</t>
+  </si>
+  <si>
+    <t>total_ahorros</t>
+  </si>
+  <si>
+    <t>Ahorros presupuestados totales durante el periodo del presupuesto</t>
   </si>
 </sst>
 </file>
@@ -921,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E7A639-BE3C-43E1-8C0C-70E76DACB4DD}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1347,7 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
@@ -1349,47 +1355,44 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1397,7 +1400,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1405,9 +1408,11 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1415,7 +1420,7 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1425,25 +1430,25 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1451,7 +1456,7 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -1461,28 +1466,25 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,17 +1492,20 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,7 +1513,7 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1518,15 +1523,15 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1534,11 +1539,9 @@
       <c r="D32" t="b">
         <v>0</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1546,25 +1549,27 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -1572,29 +1577,29 @@
       <c r="D34" t="b">
         <v>1</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1602,17 +1607,17 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1620,7 +1625,7 @@
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
@@ -1630,25 +1635,25 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1656,7 +1661,7 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -1666,28 +1671,25 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>10</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1695,7 +1697,7 @@
         <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -1704,11 +1706,11 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1716,17 +1718,20 @@
         <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>50</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1734,7 +1739,7 @@
         <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -1744,7 +1749,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,27 +1757,25 @@
         <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
         <v>157</v>
@@ -1784,25 +1787,27 @@
         <v>158</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G46" s="1" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1810,7 +1815,7 @@
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -1820,25 +1825,25 @@
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1846,7 +1851,7 @@
         <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
         <v>37</v>
@@ -1856,36 +1861,33 @@
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
-      </c>
-      <c r="E50" t="s">
-        <v>10</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1894,11 +1896,11 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1906,7 +1908,7 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
         <v>9</v>
@@ -1919,25 +1921,28 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>50</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1945,35 +1950,35 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
       </c>
       <c r="D55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1981,7 +1986,7 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
         <v>23</v>
@@ -1991,25 +1996,25 @@
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2017,7 +2022,7 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
@@ -2027,28 +2032,25 @@
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
-      </c>
-      <c r="E59" t="s">
-        <v>10</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2056,7 +2058,7 @@
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2065,19 +2067,19 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
@@ -2090,25 +2092,28 @@
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>50</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2116,7 +2121,7 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
@@ -2126,7 +2131,7 @@
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2134,17 +2139,17 @@
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2152,19 +2157,17 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2172,19 +2175,19 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2192,17 +2195,19 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G67" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2210,35 +2215,35 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" t="s">
         <v>29</v>
       </c>
       <c r="D68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2246,7 +2251,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C70" t="s">
         <v>23</v>
@@ -2256,25 +2261,25 @@
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2282,7 +2287,7 @@
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C72" t="s">
         <v>37</v>
@@ -2292,28 +2297,25 @@
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
-      </c>
-      <c r="E73" t="s">
-        <v>10</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,28 +2323,28 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -2355,25 +2357,28 @@
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C76" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>50</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2381,27 +2386,25 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
         <v>9</v>
@@ -2409,12 +2412,11 @@
       <c r="D78" t="b">
         <v>0</v>
       </c>
-      <c r="E78" t="s">
-        <v>50</v>
-      </c>
-      <c r="F78" s="1"/>
+      <c r="F78" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G78" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2422,20 +2424,20 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" t="s">
         <v>50</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2443,27 +2445,28 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D80" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>50</v>
+      </c>
+      <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
         <v>23</v>
@@ -2471,9 +2474,11 @@
       <c r="D81" t="b">
         <v>0</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G81" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2481,17 +2486,17 @@
         <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C82" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2499,109 +2504,109 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D85" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G85" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>76</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>18</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2609,7 +2614,7 @@
         <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C89" t="s">
         <v>23</v>
@@ -2619,25 +2624,25 @@
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C90" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2645,7 +2650,7 @@
         <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C91" t="s">
         <v>37</v>
@@ -2655,28 +2660,25 @@
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
-      </c>
-      <c r="E92" t="s">
-        <v>10</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2684,7 +2686,7 @@
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2693,19 +2695,19 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C94" t="s">
         <v>9</v>
@@ -2718,25 +2720,28 @@
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C95" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>50</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2744,7 +2749,7 @@
         <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C96" t="s">
         <v>23</v>
@@ -2754,7 +2759,7 @@
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2762,25 +2767,25 @@
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C97" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
@@ -2790,33 +2795,33 @@
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>88</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s">
         <v>29</v>
@@ -2826,7 +2831,7 @@
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2834,27 +2839,25 @@
         <v>88</v>
       </c>
       <c r="B101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C101" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>88</v>
       </c>
       <c r="B102" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
@@ -2863,18 +2866,18 @@
         <v>0</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -2882,9 +2885,11 @@
       <c r="D103" t="b">
         <v>0</v>
       </c>
-      <c r="F103" s="1"/>
+      <c r="F103" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="G103" s="1" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2892,7 +2897,7 @@
         <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C104" t="s">
         <v>23</v>
@@ -2902,25 +2907,25 @@
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>88</v>
       </c>
       <c r="B105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C105" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2928,7 +2933,7 @@
         <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C106" t="s">
         <v>37</v>
@@ -2938,12 +2943,26 @@
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>88</v>
+      </c>
+      <c r="B107" t="s">
+        <v>36</v>
+      </c>
+      <c r="C107" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F108" s="1"/>
@@ -3007,12 +3026,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3166,15 +3182,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3198,17 +3225,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CE08172-66DD-4532-95C5-DE15736FBE28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B847C33D-4851-4DC0-9535-7A9ECE633B56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="76cacb90-fab5-4ebd-b504-b341093fce80"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>